<commit_message>
Weight and Balance Update
Upated wing CD0 values
Fixed LG placement
Adjusted CG Excursion Diagram
</commit_message>
<xml_diff>
--- a/CG_Calc_Copy.xlsx
+++ b/CG_Calc_Copy.xlsx
@@ -9,13 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ZCG" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="101">
   <si>
     <t>Component</t>
   </si>
@@ -254,9 +258,6 @@
     <t>MTOW - Max Payload</t>
   </si>
   <si>
-    <t>MTOW - Max Payload - Fuel</t>
-  </si>
-  <si>
     <t>Wing Geometry</t>
   </si>
   <si>
@@ -291,17 +292,81 @@
   </si>
   <si>
     <t>CG Range (% MAC)</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>XAC</t>
+  </si>
+  <si>
+    <t>LG Location</t>
+  </si>
+  <si>
+    <t>B=</t>
+  </si>
+  <si>
+    <t>ft, wheel base</t>
+  </si>
+  <si>
+    <t>ft, from nose to nose gear</t>
+  </si>
+  <si>
+    <t>Nose Gear=</t>
+  </si>
+  <si>
+    <t>CO=</t>
+  </si>
+  <si>
+    <t>ft, dist between MG and AFT CG</t>
+  </si>
+  <si>
+    <t>Loading Scenario</t>
+  </si>
+  <si>
+    <t>Operating Empty Weight</t>
+  </si>
+  <si>
+    <t>Operating Empty Weight + Payload</t>
+  </si>
+  <si>
+    <t>Empty Weight</t>
+  </si>
+  <si>
+    <t>Maximum Takeoff Weight (MTOW)</t>
+  </si>
+  <si>
+    <t>Location of ZCG (ft)</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Moment</t>
+  </si>
+  <si>
+    <t>Zcg (ft)</t>
+  </si>
+  <si>
+    <t>MTOW - PAX (With Baggage)</t>
+  </si>
+  <si>
+    <t>MTOW - PAX - Typical Fuel</t>
+  </si>
+  <si>
+    <t>MTOW - Max Payload - Typical Fuel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,8 +403,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +420,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -398,9 +475,6 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -412,9 +486,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -448,12 +519,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -463,8 +528,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,6 +632,27 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="11">
+          <cell r="F11">
+            <v>90.88</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -837,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F2:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView topLeftCell="F7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,37 +984,37 @@
       </c>
     </row>
     <row r="4" spans="6:17" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="15" t="s">
         <v>16</v>
       </c>
     </row>
@@ -906,35 +1023,35 @@
         <v>4</v>
       </c>
       <c r="G5" s="6">
-        <v>4137.8</v>
-      </c>
-      <c r="H5" s="7">
+        <v>4122.8</v>
+      </c>
+      <c r="H5" s="32">
         <f>80+5.3446</f>
         <v>85.3446</v>
       </c>
       <c r="I5" s="6">
         <f>G5*H5</f>
-        <v>353138.88588000002</v>
+        <v>351858.71688000002</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="6">
         <f>$O$5*(G11/(G11+G12))</f>
-        <v>151.09083518650215</v>
-      </c>
-      <c r="L5" s="7">
+        <v>150.75478887097788</v>
+      </c>
+      <c r="L5" s="32">
         <v>32</v>
       </c>
       <c r="M5" s="6">
         <f>K5*L5</f>
-        <v>4834.9067259680687</v>
+        <v>4824.153243871292</v>
       </c>
       <c r="O5" s="6">
-        <v>1139.2</v>
+        <v>1136</v>
       </c>
       <c r="P5" s="6">
-        <v>3218</v>
+        <v>3209</v>
       </c>
       <c r="Q5" s="6">
         <v>13950</v>
@@ -945,28 +1062,28 @@
         <v>6</v>
       </c>
       <c r="G6" s="6">
-        <v>7674.8</v>
-      </c>
-      <c r="H6" s="7">
-        <v>65</v>
+        <v>7666.3</v>
+      </c>
+      <c r="H6" s="32">
+        <v>61</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" ref="I6:I16" si="0">G6*H6</f>
-        <v>498862</v>
-      </c>
-      <c r="J6" s="8" t="s">
+        <v>467644.3</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="6">
         <f>$O$5*(G12/(G12+G11))</f>
-        <v>988.10916481349796</v>
-      </c>
-      <c r="L6" s="7">
-        <v>94.68</v>
+        <v>985.24521112902221</v>
+      </c>
+      <c r="L6" s="32">
+        <v>94.75</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" ref="M6:M14" si="1">K6*L6</f>
-        <v>93554.175724541987</v>
+        <v>93351.983754474859</v>
       </c>
     </row>
     <row r="7" spans="6:17" x14ac:dyDescent="0.25">
@@ -974,28 +1091,28 @@
         <v>8</v>
       </c>
       <c r="G7" s="6">
-        <v>1048.5</v>
-      </c>
-      <c r="H7" s="7">
+        <v>996.68</v>
+      </c>
+      <c r="H7" s="32">
         <f>80+5.3446+6.25+46.7593+(0.25*11.2)</f>
         <v>141.15390000000002</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="0"/>
-        <v>147999.86415000001</v>
+        <v>140685.26905200002</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="K7" s="6">
-        <v>1105.0999999999999</v>
-      </c>
-      <c r="L7" s="7">
+        <v>1102.0999999999999</v>
+      </c>
+      <c r="L7" s="32">
         <v>26.83</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="1"/>
-        <v>29649.832999999995</v>
+        <v>29569.342999999997</v>
       </c>
     </row>
     <row r="8" spans="6:17" x14ac:dyDescent="0.25">
@@ -1003,49 +1120,49 @@
         <v>10</v>
       </c>
       <c r="G8" s="6">
-        <v>483.11329999999998</v>
-      </c>
-      <c r="H8" s="7">
+        <v>459</v>
+      </c>
+      <c r="H8" s="32">
         <f>80+5.3446+6.25+46.7593+(0.25*11.2)</f>
         <v>141.15390000000002</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="0"/>
-        <v>68193.326436870004</v>
+        <v>64789.640100000011</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="6">
-        <v>1878.2</v>
-      </c>
-      <c r="L8" s="7">
+        <v>1875.9</v>
+      </c>
+      <c r="L8" s="32">
         <v>28</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="1"/>
-        <v>52589.599999999999</v>
-      </c>
-      <c r="O8" s="30" t="s">
+        <v>52525.200000000004</v>
+      </c>
+      <c r="O8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
     </row>
     <row r="9" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="6">
         <f>P5-P5/3</f>
-        <v>2145.333333333333</v>
-      </c>
-      <c r="H9" s="7">
+        <v>2139.333333333333</v>
+      </c>
+      <c r="H9" s="32">
         <v>121.2925</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="0"/>
-        <v>260212.84333333329</v>
+        <v>259485.08833333332</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>11</v>
@@ -1053,35 +1170,35 @@
       <c r="K9" s="6">
         <v>411.24860000000001</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="32">
         <v>138.47999999999999</v>
       </c>
       <c r="M9" s="6">
         <f t="shared" si="1"/>
         <v>56949.706127999998</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="O9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="29">
-        <v>87182</v>
-      </c>
-      <c r="Q9" s="29"/>
+      <c r="P9" s="38">
+        <v>86931</v>
+      </c>
+      <c r="Q9" s="38"/>
     </row>
     <row r="10" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <f>P5/3</f>
-        <v>1072.6666666666667</v>
-      </c>
-      <c r="H10" s="11">
+        <v>1069.6666666666667</v>
+      </c>
+      <c r="H10" s="33">
         <v>141.4092</v>
       </c>
       <c r="I10" s="6">
         <f t="shared" si="0"/>
-        <v>151684.93520000001</v>
+        <v>151260.70760000002</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>13</v>
@@ -1089,70 +1206,70 @@
       <c r="K10" s="6">
         <v>40.057400000000001</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="32">
         <v>41.167000000000002</v>
       </c>
       <c r="M10" s="6">
         <f t="shared" si="1"/>
         <v>1649.0429858000002</v>
       </c>
-      <c r="O10" s="19" t="s">
+      <c r="O10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="P10" s="29">
-        <v>44042</v>
-      </c>
-      <c r="Q10" s="29"/>
+      <c r="P10" s="38">
+        <v>43908</v>
+      </c>
+      <c r="Q10" s="38"/>
     </row>
     <row r="11" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="6">
-        <v>317.59210000000002</v>
-      </c>
-      <c r="H11" s="7">
-        <v>32</v>
+        <v>316.95</v>
+      </c>
+      <c r="H11" s="32">
+        <v>31</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" si="0"/>
-        <v>10162.947200000001</v>
+        <v>9825.4499999999989</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K11" s="6">
-        <v>438.15170000000001</v>
-      </c>
-      <c r="L11" s="7">
+        <v>436.9273</v>
+      </c>
+      <c r="L11" s="32">
         <v>135</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" si="1"/>
-        <v>59150.479500000001</v>
-      </c>
-      <c r="O11" s="19" t="s">
+        <v>58985.1855</v>
+      </c>
+      <c r="O11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="29">
+      <c r="P11" s="38">
         <f>K15</f>
-        <v>43641.814799999993</v>
-      </c>
-      <c r="Q11" s="29"/>
+        <v>43508.290600000008</v>
+      </c>
+      <c r="Q11" s="38"/>
     </row>
     <row r="12" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="6">
-        <v>2077</v>
-      </c>
-      <c r="H12" s="7">
-        <v>94.68</v>
+        <v>2071.4</v>
+      </c>
+      <c r="H12" s="32">
+        <v>94.75</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" si="0"/>
-        <v>196650.36000000002</v>
+        <v>196265.15</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>17</v>
@@ -1160,30 +1277,30 @@
       <c r="K12" s="6">
         <v>756</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="32">
         <v>41.167000000000002</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" si="1"/>
         <v>31122.252</v>
       </c>
-      <c r="O12" s="19" t="s">
+      <c r="O12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="29">
-        <v>40991</v>
-      </c>
-      <c r="Q12" s="29"/>
+      <c r="P12" s="38">
+        <v>40872</v>
+      </c>
+      <c r="Q12" s="38"/>
     </row>
     <row r="13" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <f>Q5-Q5/3</f>
         <v>9300</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="33">
         <v>119.55</v>
       </c>
       <c r="I13" s="6">
@@ -1196,7 +1313,7 @@
       <c r="K13" s="6">
         <v>280</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="32">
         <v>30.5</v>
       </c>
       <c r="M13" s="6">
@@ -1205,14 +1322,14 @@
       </c>
     </row>
     <row r="14" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <f>Q5/3</f>
         <v>4650</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="33">
         <v>140.85</v>
       </c>
       <c r="I14" s="6">
@@ -1223,82 +1340,82 @@
         <v>21</v>
       </c>
       <c r="K14" s="6">
-        <v>438.15170000000001</v>
-      </c>
-      <c r="L14" s="7">
+        <v>436.9273</v>
+      </c>
+      <c r="L14" s="32">
         <v>75.2</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" si="1"/>
-        <v>32949.007839999998</v>
+        <v>32856.932959999998</v>
       </c>
     </row>
     <row r="15" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="10">
-        <v>1473.6</v>
-      </c>
-      <c r="H15" s="12">
-        <f>Sheet2!F11</f>
+      <c r="G15" s="9">
+        <v>1470.2</v>
+      </c>
+      <c r="H15" s="34">
+        <f>[1]Sheet2!F11</f>
         <v>90.88</v>
       </c>
       <c r="I15" s="6">
         <f t="shared" si="0"/>
-        <v>133920.76799999998</v>
-      </c>
-      <c r="J15" s="13" t="s">
+        <v>133611.77599999998</v>
+      </c>
+      <c r="J15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="12">
         <f>SUM(G5:G16,K5:K14)</f>
-        <v>43641.814799999993</v>
-      </c>
-      <c r="L15" s="11"/>
-      <c r="M15" s="8"/>
+        <v>43508.290600000008</v>
+      </c>
+      <c r="L15" s="10"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G16" s="6">
-        <v>2775.3</v>
-      </c>
-      <c r="H16" s="7">
+        <v>2770.8</v>
+      </c>
+      <c r="H16" s="32">
         <v>26.83</v>
       </c>
       <c r="I16" s="6">
         <f t="shared" si="0"/>
-        <v>74461.298999999999</v>
-      </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+        <v>74340.563999999998</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="18" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="25" t="s">
         <v>43</v>
       </c>
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="24" t="s">
         <v>42</v>
       </c>
       <c r="G19">
         <v>2</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="27" t="s">
+      <c r="I19" s="25" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="24" t="s">
         <v>47</v>
       </c>
       <c r="G20">
@@ -1312,74 +1429,74 @@
         <f>G20*H20</f>
         <v>10720</v>
       </c>
-      <c r="K20" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="L20" s="36"/>
+      <c r="K20" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="37"/>
     </row>
     <row r="21" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="24" t="s">
         <v>46</v>
       </c>
       <c r="G21" s="3">
         <f>K15+G20</f>
-        <v>44041.814799999993</v>
-      </c>
-      <c r="K21" s="24" t="s">
+        <v>43908.290600000008</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L21">
+        <v>21.75</v>
+      </c>
+      <c r="M21" t="s">
         <v>75</v>
       </c>
-      <c r="L21">
-        <v>21.85</v>
-      </c>
-      <c r="M21" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="22" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="K22" s="24" t="s">
+      <c r="K22" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="L22">
+        <v>16.59</v>
+      </c>
+      <c r="M22" t="s">
         <v>71</v>
       </c>
-      <c r="L22">
-        <v>16.66</v>
-      </c>
-      <c r="M22" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="23" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="24" t="s">
-        <v>70</v>
+      <c r="K23" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="L23">
         <v>80</v>
       </c>
       <c r="M23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="24" t="s">
         <v>41</v>
       </c>
       <c r="G24">
         <v>10</v>
       </c>
-      <c r="K24" s="24" t="s">
-        <v>74</v>
+      <c r="K24" s="22" t="s">
+        <v>73</v>
       </c>
       <c r="L24">
         <f>(L21-L22)/2</f>
-        <v>2.5950000000000006</v>
+        <v>2.58</v>
       </c>
       <c r="M24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="24" t="s">
         <v>57</v>
       </c>
       <c r="G25">
@@ -1388,22 +1505,25 @@
       </c>
     </row>
     <row r="26" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="24" t="s">
         <v>56</v>
       </c>
       <c r="G26">
         <f>G24*45</f>
         <v>450</v>
       </c>
-      <c r="H26" s="27" t="s">
+      <c r="H26" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="I26" s="27" t="s">
+      <c r="I26" s="25" t="s">
         <v>3</v>
       </c>
+      <c r="K26" s="22" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="27" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="24" t="s">
         <v>55</v>
       </c>
       <c r="G27">
@@ -1417,39 +1537,69 @@
         <f>G27*H27</f>
         <v>77400</v>
       </c>
+      <c r="K27" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="L27">
+        <v>64</v>
+      </c>
+      <c r="M27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="K28" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="L28">
+        <v>31</v>
+      </c>
+      <c r="M28" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="29" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F29" s="27" t="s">
+      <c r="F29" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="H29" s="27" t="s">
+      <c r="H29" s="25" t="s">
         <v>52</v>
       </c>
+      <c r="K29" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="L29" s="28">
+        <f>(L27+L28)-I34</f>
+        <v>3.364408103464342</v>
+      </c>
+      <c r="M29" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="30" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="28">
+      <c r="G30" s="26">
         <f>P12</f>
-        <v>40991</v>
+        <v>40872</v>
       </c>
       <c r="H30">
         <v>90.9</v>
       </c>
       <c r="I30" s="3">
         <f>G30*H30</f>
-        <v>3726081.9000000004</v>
+        <v>3715264.8000000003</v>
       </c>
     </row>
     <row r="31" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="24" t="s">
         <v>54</v>
       </c>
       <c r="G31">
         <v>50000</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="23">
         <f>Sheet2!F11</f>
         <v>90.88</v>
       </c>
@@ -1457,43 +1607,56 @@
         <f>G31*H31</f>
         <v>4544000</v>
       </c>
+      <c r="N31" t="s">
+        <v>81</v>
+      </c>
+      <c r="O31">
+        <v>0.73</v>
+      </c>
     </row>
     <row r="33" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="H33" s="31" t="s">
+      <c r="H33" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I33" s="35" t="s">
+      <c r="I33" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="J33" s="31" t="s">
-        <v>78</v>
+      <c r="J33" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F34" s="33" t="s">
+      <c r="F34" s="29" t="s">
         <v>29</v>
       </c>
       <c r="G34" s="3">
         <f>K15</f>
-        <v>43641.814799999993</v>
+        <v>43508.290600000008</v>
       </c>
       <c r="H34" s="3">
         <f>SUM(I5:I16,M5:M14)</f>
-        <v>4033043.7331045135</v>
-      </c>
-      <c r="I34" s="34">
+        <v>3986907.961537479</v>
+      </c>
+      <c r="I34" s="35">
         <f>H34/G34</f>
-        <v>92.412374498791792</v>
-      </c>
-      <c r="J34" s="32">
+        <v>91.635591896535658</v>
+      </c>
+      <c r="J34" s="36">
         <f>(I34-$L$23-$L$24)/$L$22</f>
-        <v>0.58927818119998743</v>
+        <v>0.54584640726556111</v>
+      </c>
+      <c r="K34" s="28">
+        <f>O31-J34</f>
+        <v>0.18415359273443888</v>
       </c>
     </row>
     <row r="35" spans="6:12" x14ac:dyDescent="0.25">
@@ -1502,19 +1665,23 @@
       </c>
       <c r="G35" s="3">
         <f>G34+G20</f>
-        <v>44041.814799999993</v>
+        <v>43908.290600000008</v>
       </c>
       <c r="H35" s="3">
         <f>H34+I20</f>
-        <v>4043763.7331045135</v>
-      </c>
-      <c r="I35" s="34">
+        <v>3997627.961537479</v>
+      </c>
+      <c r="I35" s="30">
         <f t="shared" ref="I35:I39" si="2">H35/G35</f>
-        <v>91.816464681753175</v>
-      </c>
-      <c r="J35" s="32">
+        <v>91.044946339529744</v>
+      </c>
+      <c r="J35" s="28">
         <f t="shared" ref="J35:J39" si="3">(I35-$L$23-$L$24)/$L$22</f>
-        <v>0.55350928461903803</v>
+        <v>0.51024390232246797</v>
+      </c>
+      <c r="K35" s="28">
+        <f>O31-J35</f>
+        <v>0.21975609767753201</v>
       </c>
     </row>
     <row r="36" spans="6:12" x14ac:dyDescent="0.25">
@@ -1523,19 +1690,23 @@
       </c>
       <c r="G36" s="3">
         <f>G35+G27</f>
-        <v>46191.814799999993</v>
+        <v>46058.290600000008</v>
       </c>
       <c r="H36" s="3">
         <f>H35+I27</f>
-        <v>4121163.7331045135</v>
-      </c>
-      <c r="I36" s="34">
+        <v>4075027.961537479</v>
+      </c>
+      <c r="I36" s="30">
         <f t="shared" si="2"/>
-        <v>89.218484940420964</v>
-      </c>
-      <c r="J36" s="32">
+        <v>88.475449445739486</v>
+      </c>
+      <c r="J36" s="28">
         <f t="shared" si="3"/>
-        <v>0.39756812367472771</v>
+        <v>0.35536163024348916</v>
+      </c>
+      <c r="K36" s="28">
+        <f>O31-J36</f>
+        <v>0.37463836975651083</v>
       </c>
     </row>
     <row r="37" spans="6:12" x14ac:dyDescent="0.25">
@@ -1544,19 +1715,23 @@
       </c>
       <c r="G37" s="3">
         <f>G36+G30</f>
-        <v>87182.814799999993</v>
+        <v>86930.290600000008</v>
       </c>
       <c r="H37" s="3">
         <f>H36+I30</f>
-        <v>7847245.6331045143</v>
-      </c>
-      <c r="I37" s="34">
+        <v>7790292.7615374792</v>
+      </c>
+      <c r="I37" s="35">
         <f t="shared" si="2"/>
-        <v>90.009087812848577</v>
-      </c>
-      <c r="J37" s="32">
+        <v>89.615399968966386</v>
+      </c>
+      <c r="J37" s="36">
         <f t="shared" si="3"/>
-        <v>0.44502327808214742</v>
+        <v>0.42407474195095757</v>
+      </c>
+      <c r="K37" s="28">
+        <f>O31-J37</f>
+        <v>0.30592525804904241</v>
       </c>
     </row>
     <row r="38" spans="6:12" x14ac:dyDescent="0.25">
@@ -1565,117 +1740,125 @@
       </c>
       <c r="G38" s="3">
         <f>G37-G27</f>
-        <v>85032.814799999993</v>
+        <v>84780.290600000008</v>
       </c>
       <c r="H38" s="3">
         <f>H37-I27</f>
-        <v>7769845.6331045143</v>
-      </c>
-      <c r="I38" s="34">
+        <v>7712892.7615374792</v>
+      </c>
+      <c r="I38" s="30">
         <f t="shared" si="2"/>
-        <v>91.374672841060828</v>
-      </c>
-      <c r="J38" s="32">
+        <v>90.975068697599852</v>
+      </c>
+      <c r="J38" s="28">
         <f t="shared" si="3"/>
-        <v>0.52699116693042181</v>
+        <v>0.50603186845086512</v>
+      </c>
+      <c r="K38" s="28">
+        <f>O31-J38</f>
+        <v>0.22396813154913486</v>
       </c>
     </row>
     <row r="39" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="G39" s="3">
         <f>G38-G30</f>
-        <v>44041.814799999993</v>
+        <v>43908.290600000008</v>
       </c>
       <c r="H39" s="3">
         <f>H38-I30</f>
-        <v>4043763.733104514</v>
-      </c>
-      <c r="I39" s="34">
+        <v>3997627.961537479</v>
+      </c>
+      <c r="I39" s="30">
         <f t="shared" si="2"/>
-        <v>91.816464681753189</v>
-      </c>
-      <c r="J39" s="32">
+        <v>91.044946339529744</v>
+      </c>
+      <c r="J39" s="28">
         <f t="shared" si="3"/>
-        <v>0.55350928461903892</v>
+        <v>0.51024390232246797</v>
+      </c>
+      <c r="K39" s="28">
+        <f>O31-J39</f>
+        <v>0.21975609767753201</v>
       </c>
     </row>
     <row r="41" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>79</v>
-      </c>
-      <c r="G41" s="25">
+        <v>78</v>
+      </c>
+      <c r="G41" s="23">
         <f>MAX(I34:I39) - MIN(I34:I39)</f>
-        <v>3.1938895583708273</v>
+        <v>3.1601424507961724</v>
       </c>
     </row>
     <row r="42" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>80</v>
-      </c>
-      <c r="G42" s="32">
+        <v>79</v>
+      </c>
+      <c r="G42" s="28">
         <f>MAX(J34:J39) - MIN(J34:J39)</f>
-        <v>0.19171005752525971</v>
+        <v>0.19048477702207195</v>
       </c>
     </row>
     <row r="46" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="L46" s="20"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="L46" s="18"/>
     </row>
     <row r="47" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="L47" s="20"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="L47" s="18"/>
     </row>
     <row r="48" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F48" s="2"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
     </row>
     <row r="49" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F49" s="2"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
     </row>
     <row r="50" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F50" s="2"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
     </row>
     <row r="51" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F51" s="2"/>
       <c r="G51" s="1"/>
       <c r="H51" s="4"/>
-      <c r="I51" s="23"/>
-      <c r="J51" s="23"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
     </row>
     <row r="52" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F52" s="2"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="23"/>
-      <c r="I52" s="23"/>
-      <c r="J52" s="23"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
     </row>
     <row r="53" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F53" s="2"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1695,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,7 +2040,7 @@
       </c>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>39</v>
       </c>
       <c r="F9">
@@ -1881,14 +2064,14 @@
       <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="23">
         <f>G9/F9</f>
         <v>90.88</v>
       </c>
       <c r="I11" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="23">
         <f>L9/K9</f>
         <v>90.880973872313433</v>
       </c>
@@ -1897,4 +2080,623 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:J39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34:F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:10" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4122.8</v>
+      </c>
+      <c r="E5" s="40">
+        <v>1.0848</v>
+      </c>
+      <c r="F5" s="6">
+        <f>D5*E5</f>
+        <v>4472.4134400000003</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="6">
+        <v>150.75478887097788</v>
+      </c>
+      <c r="I5" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="J5" s="6">
+        <f>H5*I5</f>
+        <v>226.1321833064668</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6">
+        <v>7666.3</v>
+      </c>
+      <c r="E6" s="32">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" ref="F6:F16" si="0">D6*E6</f>
+        <v>31815.145000000004</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6">
+        <v>985.24521112902221</v>
+      </c>
+      <c r="I6" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" ref="J6:J16" si="1">H6*I6</f>
+        <v>1477.8678166935333</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6">
+        <v>996.68</v>
+      </c>
+      <c r="E7" s="32">
+        <v>20.71</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="0"/>
+        <v>20641.2428</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1102.0999999999999</v>
+      </c>
+      <c r="I7" s="32">
+        <v>6.25</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="1"/>
+        <v>6888.1249999999991</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6">
+        <v>459</v>
+      </c>
+      <c r="E8" s="32">
+        <v>12.3421</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="0"/>
+        <v>5665.0239000000001</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1875.9</v>
+      </c>
+      <c r="I8" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>4689.75</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2139.333333333333</v>
+      </c>
+      <c r="E9" s="42">
+        <v>5.2916999999999996</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="0"/>
+        <v>11320.710199999998</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6">
+        <v>411.24860000000001</v>
+      </c>
+      <c r="I9" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="1"/>
+        <v>1850.6187</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1069.6666666666667</v>
+      </c>
+      <c r="E10" s="41">
+        <v>7</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="0"/>
+        <v>7487.666666666667</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="6">
+        <v>40.057400000000001</v>
+      </c>
+      <c r="I10" s="32">
+        <v>7</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="1"/>
+        <v>280.40179999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="6">
+        <v>316.95</v>
+      </c>
+      <c r="E11" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="0"/>
+        <v>475.42499999999995</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="6">
+        <v>436.9273</v>
+      </c>
+      <c r="I11" s="32">
+        <v>5.3</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="1"/>
+        <v>2315.7146899999998</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2071.4</v>
+      </c>
+      <c r="E12" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="0"/>
+        <v>3107.1000000000004</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="6">
+        <v>756</v>
+      </c>
+      <c r="I12" s="32">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="1"/>
+        <v>3137.4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="9">
+        <v>9300</v>
+      </c>
+      <c r="E13" s="42">
+        <v>5.2916999999999996</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="0"/>
+        <v>49212.81</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="6">
+        <v>280</v>
+      </c>
+      <c r="I13" s="32">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="1"/>
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="9">
+        <v>4650</v>
+      </c>
+      <c r="E14" s="41">
+        <v>7</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="0"/>
+        <v>32550</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="6">
+        <v>436.9273</v>
+      </c>
+      <c r="I14" s="32">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="1"/>
+        <v>1813.2482950000001</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1470.2</v>
+      </c>
+      <c r="E15" s="34">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="0"/>
+        <v>6101.3300000000008</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="12">
+        <v>43508.290600000008</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2770.8</v>
+      </c>
+      <c r="E16" s="32">
+        <v>5.4166999999999996</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="0"/>
+        <v>15008.592360000001</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <f>D18*(170+30)</f>
+        <v>400</v>
+      </c>
+      <c r="E19">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F19">
+        <f>D19*E19</f>
+        <v>1660.0000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3">
+        <f>H15+D19</f>
+        <v>43908.290600000008</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24">
+        <f>D23*170</f>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25">
+        <f>D23*45</f>
+        <v>450</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26">
+        <f>D24+D25</f>
+        <v>2150</v>
+      </c>
+      <c r="E26">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F26" s="3">
+        <f>D26*E26</f>
+        <v>8922.5</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="26">
+        <v>40872</v>
+      </c>
+      <c r="E29" s="28">
+        <v>6</v>
+      </c>
+      <c r="F29" s="3">
+        <f>D29*E29</f>
+        <v>245232</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30">
+        <v>50000</v>
+      </c>
+      <c r="E30" s="28">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <f>D30*E30</f>
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="3">
+        <f>H15</f>
+        <v>43508.290600000008</v>
+      </c>
+      <c r="E34" s="3">
+        <f>SUM(F5:F16,J5:J14)</f>
+        <v>211698.71785166665</v>
+      </c>
+      <c r="F34" s="28">
+        <f>E34/D34</f>
+        <v>4.8657098436238408</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="3">
+        <f>D20</f>
+        <v>43908.290600000008</v>
+      </c>
+      <c r="E35" s="3">
+        <f>E34+F19</f>
+        <v>213358.71785166665</v>
+      </c>
+      <c r="F35" s="28">
+        <f t="shared" ref="F35:F39" si="2">E35/D35</f>
+        <v>4.8591898007449785</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="3">
+        <f>D35+D26</f>
+        <v>46058.290600000008</v>
+      </c>
+      <c r="E36" s="3">
+        <f>E35+F26</f>
+        <v>222281.21785166665</v>
+      </c>
+      <c r="F36" s="28">
+        <f t="shared" si="2"/>
+        <v>4.8260848363240516</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="3">
+        <f>40872+D36</f>
+        <v>86930.290600000008</v>
+      </c>
+      <c r="E37" s="3">
+        <f>E36+F29</f>
+        <v>467513.21785166662</v>
+      </c>
+      <c r="F37" s="28">
+        <f t="shared" si="2"/>
+        <v>5.3780243298952755</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C38" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="3">
+        <f>D37-D26</f>
+        <v>84780.290600000008</v>
+      </c>
+      <c r="E38" s="3">
+        <f>E37-F26</f>
+        <v>458590.71785166662</v>
+      </c>
+      <c r="F38" s="28">
+        <f t="shared" si="2"/>
+        <v>5.4091666188705725</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C39" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="3">
+        <f>D38-D29</f>
+        <v>43908.290600000008</v>
+      </c>
+      <c r="E39" s="3">
+        <f>E38-F29</f>
+        <v>213358.71785166662</v>
+      </c>
+      <c r="F39" s="28">
+        <f t="shared" si="2"/>
+        <v>4.8591898007449776</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>